<commit_message>
Fix date comptabilisation issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_6_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_6_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,7 +423,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>002/DR002</v>
+        <v>098/TTTTT</v>
       </c>
       <c r="B2" t="str">
         <v>Direction régionale</v>
@@ -444,54 +444,54 @@
         <v>15</v>
       </c>
       <c r="H2">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>7500</v>
+        <v>1500</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>92500</v>
+        <v>8500</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>794/DR KESH</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B3" t="str">
-        <v>Direction régionale</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C3" t="str">
-        <v>KS10293</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D3" t="str">
-        <v>Karim benzima</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E3" t="str">
-        <v>non</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F3" t="str">
-        <v>annuelle</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G3" t="str">
+        <v xml:space="preserve"> </v>
       </c>
       <c r="H3">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>10000</v>
+        <v>1500</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -500,53 +500,12 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>90000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="B4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H4">
-        <v>200000</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>17500</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>50000</v>
-      </c>
-      <c r="M4">
-        <v>182500</v>
+        <v>8500</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix annex 2 and update av issues
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_6_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_6_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,34 +423,34 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>844/T-SUD</v>
+        <v>001/LF/TEST DR/AV1</v>
       </c>
       <c r="B2" t="str">
-        <v>Point de vente</v>
+        <v>Logement de fonction</v>
       </c>
       <c r="C2" t="str">
-        <v>K324554</v>
+        <v>11986345</v>
       </c>
       <c r="D2" t="str">
-        <v>KARIMA SASA</v>
+        <v>ALI EXPRESSE</v>
       </c>
       <c r="E2" t="str">
-        <v>non</v>
+        <v>oui</v>
       </c>
       <c r="F2" t="str">
         <v>mensuelle</v>
       </c>
       <c r="G2">
-        <v>15</v>
-      </c>
-      <c r="H2">
-        <v>24000</v>
+        <v>0</v>
+      </c>
+      <c r="H2" t="str">
+        <v>--</v>
       </c>
       <c r="I2">
+        <v>30000</v>
+      </c>
+      <c r="J2">
         <v>0</v>
-      </c>
-      <c r="J2">
-        <v>3600</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -459,21 +459,21 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>20400</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>844/T-SUD</v>
+        <v>001/TEST DR</v>
       </c>
       <c r="B3" t="str">
-        <v>Point de vente</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C3" t="str">
-        <v>IL12254</v>
+        <v>BG432432</v>
       </c>
       <c r="D3" t="str">
-        <v>FARIDA VAVA</v>
+        <v>TETS TESTS</v>
       </c>
       <c r="E3" t="str">
         <v>non</v>
@@ -482,57 +482,57 @@
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H3">
-        <v>6000</v>
+        <v>20000</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="J3">
-        <v>600</v>
+        <v>3000</v>
       </c>
       <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
+        <v>3000</v>
+      </c>
+      <c r="L3" t="str">
+        <v>--</v>
       </c>
       <c r="M3">
-        <v>5400</v>
+        <v>17000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>115/TANGER MED/AV1</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B4" t="str">
-        <v>Point de vente</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C4" t="str">
-        <v>L5245475</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D4" t="str">
-        <v>MORAD JOJO</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E4" t="str">
-        <v>non</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F4" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G4" t="str">
+        <v xml:space="preserve"> </v>
       </c>
       <c r="H4">
-        <v>9000</v>
+        <v>20000</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="J4">
-        <v>900</v>
+        <v>3000</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -541,299 +541,12 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>8100</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>115/TANGER MED/AV1</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Point de vente</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Z213568</v>
-      </c>
-      <c r="D5" t="str">
-        <v>NABIL MOMO</v>
-      </c>
-      <c r="E5" t="str">
-        <v>non</v>
-      </c>
-      <c r="F5" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5">
-        <v>6000</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>600</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>115/TANGER MED/AV1</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Point de vente</v>
-      </c>
-      <c r="C6" t="str">
-        <v>L525655</v>
-      </c>
-      <c r="D6" t="str">
-        <v>KHALID RARA</v>
-      </c>
-      <c r="E6" t="str">
-        <v>non</v>
-      </c>
-      <c r="F6" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6">
-        <v>6000</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>600</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v xml:space="preserve">910/TANGER </v>
-      </c>
-      <c r="B7" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C7" t="str">
-        <v>D235689</v>
-      </c>
-      <c r="D7" t="str">
-        <v>KAMILIA LALA</v>
-      </c>
-      <c r="E7" t="str">
-        <v>non</v>
-      </c>
-      <c r="F7" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G7">
-        <v>15</v>
-      </c>
-      <c r="H7">
-        <v>24000</v>
-      </c>
-      <c r="I7">
-        <v>24000</v>
-      </c>
-      <c r="J7">
-        <v>3600</v>
-      </c>
-      <c r="K7">
-        <v>3600</v>
-      </c>
-      <c r="L7" t="str">
-        <v>--</v>
-      </c>
-      <c r="M7">
-        <v>20400</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v xml:space="preserve">910/TANGER </v>
-      </c>
-      <c r="B8" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Z213568</v>
-      </c>
-      <c r="D8" t="str">
-        <v>NABIL MOMO</v>
-      </c>
-      <c r="E8" t="str">
-        <v>oui</v>
-      </c>
-      <c r="F8" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>16000</v>
-      </c>
-      <c r="I8">
-        <v>16000</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8" t="str">
-        <v>--</v>
-      </c>
-      <c r="M8">
-        <v>16000</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v xml:space="preserve">910/LF/TANGER </v>
-      </c>
-      <c r="B9" t="str">
-        <v>Logement de fonction</v>
-      </c>
-      <c r="C9" t="str">
-        <v>35464645</v>
-      </c>
-      <c r="D9" t="str">
-        <v>STÉ LOCATION 1</v>
-      </c>
-      <c r="E9" t="str">
-        <v>oui</v>
-      </c>
-      <c r="F9" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>14161.71</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9" t="str">
-        <v>--</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v xml:space="preserve">910/LF/TANGER </v>
-      </c>
-      <c r="B10" t="str">
-        <v>Logement de fonction</v>
-      </c>
-      <c r="C10" t="str">
-        <v>L5245475</v>
-      </c>
-      <c r="D10" t="str">
-        <v>MORAD JOJO</v>
-      </c>
-      <c r="E10" t="str">
-        <v>non</v>
-      </c>
-      <c r="F10" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>5838.29</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10" t="str">
-        <v>--</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="B11" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C11" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D11" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E11" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F11" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G11" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H11">
-        <v>111000</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>9900</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>81100</v>
+        <v>47000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>